<commit_message>
Redigned BF109 technology-tree proposal
</commit_message>
<xml_diff>
--- a/BICE modfile/Air-research-HOI3.xlsx
+++ b/BICE modfile/Air-research-HOI3.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\maver\Documents\Paradox Interactive\Hearts of Iron IV\mod\Blackice-WIP-v2.5\BICE modfile\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{CA252DDD-574C-444D-B2E9-19468B04DC1A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{7D422950-EA43-4C3B-B885-066D2E8576A1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18180" windowHeight="8760" xr2:uid="{6F6A277D-F146-4689-B39C-DDE0518F87C0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18180" windowHeight="8760" activeTab="1" xr2:uid="{6F6A277D-F146-4689-B39C-DDE0518F87C0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="HOI3" sheetId="1" r:id="rId1"/>
+    <sheet name="HOI4" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="88">
   <si>
     <t>Single engine airframe</t>
   </si>
@@ -100,13 +101,202 @@
   </si>
   <si>
     <t>Carrier Aircraft</t>
+  </si>
+  <si>
+    <t>Aero-engine-1</t>
+  </si>
+  <si>
+    <t>tech_me_109_fighter_equipment_1</t>
+  </si>
+  <si>
+    <t>bf109-A/B</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Aero-engine-2</t>
+  </si>
+  <si>
+    <t>661hp</t>
+  </si>
+  <si>
+    <t>Jumo210D</t>
+  </si>
+  <si>
+    <t>690Hp</t>
+  </si>
+  <si>
+    <t>Jumo 210G</t>
+  </si>
+  <si>
+    <t>strenghtened wing</t>
+  </si>
+  <si>
+    <t>bf109-C</t>
+  </si>
+  <si>
+    <t>production started spring 1938; 58 109C were build</t>
+  </si>
+  <si>
+    <t>Aero-engine-3</t>
+  </si>
+  <si>
+    <t>1006 Hp</t>
+  </si>
+  <si>
+    <t>DB601A-1</t>
+  </si>
+  <si>
+    <t>2 MG17 above engine and 1 MG FF canon in each wing</t>
+  </si>
+  <si>
+    <t>438 were build</t>
+  </si>
+  <si>
+    <t>bf109-E4/E7</t>
+  </si>
+  <si>
+    <t>DB601E</t>
+  </si>
+  <si>
+    <t>droptank</t>
+  </si>
+  <si>
+    <t>300L fueltank</t>
+  </si>
+  <si>
+    <t>15MG151 cannon (200 rounds) + 2 MG17</t>
+  </si>
+  <si>
+    <t>bf109-F2</t>
+  </si>
+  <si>
+    <t>DB601N</t>
+  </si>
+  <si>
+    <t>1150 Hp</t>
+  </si>
+  <si>
+    <t>1230 were build between oct 1940 and august 1941</t>
+  </si>
+  <si>
+    <t>max speed 615km</t>
+  </si>
+  <si>
+    <t>bf109-E1/E3</t>
+  </si>
+  <si>
+    <t>1183 E1 and 1276 E3 were build</t>
+  </si>
+  <si>
+    <t>max range 1700km</t>
+  </si>
+  <si>
+    <t>max range 660km</t>
+  </si>
+  <si>
+    <t>max range 1325km</t>
+  </si>
+  <si>
+    <t>with droptank</t>
+  </si>
+  <si>
+    <t>Aero-engine-4</t>
+  </si>
+  <si>
+    <t>Aero-engine-5</t>
+  </si>
+  <si>
+    <t>1332 Hp</t>
+  </si>
+  <si>
+    <t>DB605A</t>
+  </si>
+  <si>
+    <t>1455 Hp</t>
+  </si>
+  <si>
+    <t>bf109-G1/G2</t>
+  </si>
+  <si>
+    <t>G2 production started may 1942. 1586 G2 were built</t>
+  </si>
+  <si>
+    <t>Pressurized cabin</t>
+  </si>
+  <si>
+    <t>max speed 660</t>
+  </si>
+  <si>
+    <t>underwings 20mm G 151/20 cannon gondolas</t>
+  </si>
+  <si>
+    <t>basic armament</t>
+  </si>
+  <si>
+    <t>Fug 16 VHF radioset</t>
+  </si>
+  <si>
+    <t>bf109-G4</t>
+  </si>
+  <si>
+    <t>Up to july 1943 1242 were build</t>
+  </si>
+  <si>
+    <t>13 mm MG 131 replaced the smaller MG 17</t>
+  </si>
+  <si>
+    <t>bf109-G6</t>
+  </si>
+  <si>
+    <t>Aero-engine-6</t>
+  </si>
+  <si>
+    <t>Aero-engine-7</t>
+  </si>
+  <si>
+    <t>DB 605 DB/DC</t>
+  </si>
+  <si>
+    <t>2000PS</t>
+  </si>
+  <si>
+    <t>max speed with booster and using MW 50 710km. Without MW50 670km</t>
+  </si>
+  <si>
+    <t>bf109-K4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FuG 25a Erstling IFF system</t>
+  </si>
+  <si>
+    <t>EZ 42 Gyro gunsight</t>
+  </si>
+  <si>
+    <t>30mm MK108 Motorkannone</t>
+  </si>
+  <si>
+    <t>2 MG131</t>
+  </si>
+  <si>
+    <t>underwing MG151/20 or 21cm Wfr.Gr 21 rockets</t>
+  </si>
+  <si>
+    <t>1593 produced by end march 1945</t>
+  </si>
+  <si>
+    <t>After this JETS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +312,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -131,7 +328,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -165,11 +362,137 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -178,18 +501,83 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -508,7 +896,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8729C2AD-2EED-427D-AF84-8D83C7BA7D09}">
   <dimension ref="B1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
@@ -527,14 +915,14 @@
       </c>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7"/>
+      <c r="C3" s="8"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
       <c r="D4" t="s">
         <v>10</v>
       </c>
@@ -546,87 +934,87 @@
       </c>
     </row>
     <row r="5" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="G5" s="3" t="s">
+      <c r="E5" s="6"/>
+      <c r="G5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H5" s="4"/>
-      <c r="J5" s="3" t="s">
+      <c r="H5" s="6"/>
+      <c r="J5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="4"/>
+      <c r="K5" s="6"/>
     </row>
     <row r="6" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="6"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="1">
         <v>12</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="6"/>
-      <c r="J7" s="5" t="s">
+      <c r="H7" s="4"/>
+      <c r="J7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="K7" s="6"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="G9" s="5" t="s">
+      <c r="E9" s="4"/>
+      <c r="G9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H9" s="6"/>
-      <c r="J9" s="5" t="s">
+      <c r="H9" s="4"/>
+      <c r="J9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K9" s="6"/>
+      <c r="K9" s="4"/>
     </row>
     <row r="10" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="11" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G11" s="5" t="s">
+      <c r="G11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H11" s="6"/>
+      <c r="H11" s="4"/>
       <c r="M11" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="8"/>
     </row>
     <row r="13" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
     </row>
     <row r="14" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="6"/>
+      <c r="E14" s="4"/>
       <c r="F14" s="1">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="6"/>
+      <c r="E16" s="4"/>
       <c r="F16" s="1">
         <v>12</v>
       </c>
@@ -640,10 +1028,10 @@
       </c>
     </row>
     <row r="18" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="6"/>
+      <c r="E18" s="4"/>
       <c r="G18" t="s">
         <v>0</v>
       </c>
@@ -654,10 +1042,10 @@
       </c>
     </row>
     <row r="20" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="6"/>
+      <c r="E20" s="4"/>
       <c r="G20" t="s">
         <v>3</v>
       </c>
@@ -668,24 +1056,25 @@
       </c>
     </row>
     <row r="22" spans="4:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D22" s="3" t="s">
+      <c r="D22" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="4"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="24" spans="4:7" x14ac:dyDescent="0.25">
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="2"/>
+      <c r="E24" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="B12:C13"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="G9:H9"/>
@@ -693,12 +1082,898 @@
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="J7:K7"/>
     <mergeCell ref="J9:K9"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="B12:C13"/>
-    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="D16:E16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD7AC1B-AA8B-48EB-91C0-6CDFF3EAA1E2}">
+  <dimension ref="A1:V66"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="H64" sqref="H64"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+    <col min="7" max="8" width="18.42578125" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" customWidth="1"/>
+    <col min="10" max="10" width="18.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1935</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="11"/>
+      <c r="E2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="12"/>
+      <c r="C3" s="13"/>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>1936</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="14"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>1937</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="11"/>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="12"/>
+      <c r="C12" s="13"/>
+      <c r="E12" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="H12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>1938</v>
+      </c>
+      <c r="C16" s="16"/>
+      <c r="D16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="14"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="I16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>1939</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="11"/>
+    </row>
+    <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="12"/>
+      <c r="C19" s="13"/>
+      <c r="E19" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="H19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="23"/>
+    </row>
+    <row r="21" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="22"/>
+      <c r="E21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F21" s="4"/>
+      <c r="H21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>1939</v>
+      </c>
+      <c r="C23" s="16"/>
+      <c r="D23" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="14"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="I23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>1940</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="E25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="12"/>
+      <c r="C26" s="13"/>
+      <c r="H26" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="23"/>
+      <c r="E27" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F27" s="4"/>
+      <c r="H27" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I27" s="6"/>
+      <c r="J27" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="C28" s="22"/>
+    </row>
+    <row r="29" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>1940</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="14"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="I29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>1941</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="11"/>
+      <c r="H31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="12"/>
+      <c r="C32" s="13"/>
+      <c r="E32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F32" s="6"/>
+      <c r="H32" t="s">
+        <v>55</v>
+      </c>
+      <c r="J32" t="s">
+        <v>58</v>
+      </c>
+      <c r="L32" s="2"/>
+    </row>
+    <row r="33" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="C33" s="23"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
+      <c r="J33" s="17"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="18"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="17"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="17"/>
+      <c r="Q33" s="17"/>
+      <c r="R33" s="17"/>
+      <c r="S33" s="17"/>
+      <c r="T33" s="17"/>
+      <c r="U33" s="17"/>
+      <c r="V33" s="17"/>
+    </row>
+    <row r="34" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C34" s="22"/>
+      <c r="E34" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F34" s="4"/>
+      <c r="H34" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="17"/>
+      <c r="S34" s="17"/>
+      <c r="T34" s="17"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="17"/>
+    </row>
+    <row r="35" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="17"/>
+      <c r="N35" s="17"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="17"/>
+      <c r="Q35" s="17"/>
+      <c r="R35" s="17"/>
+      <c r="S35" s="17"/>
+      <c r="T35" s="17"/>
+      <c r="U35" s="17"/>
+      <c r="V35" s="17"/>
+    </row>
+    <row r="36" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>1941</v>
+      </c>
+      <c r="C36" s="16"/>
+      <c r="D36" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E36" s="14"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="17"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
+      <c r="R36" s="17"/>
+      <c r="S36" s="17"/>
+      <c r="T36" s="17"/>
+      <c r="U36" s="17"/>
+      <c r="V36" s="17"/>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H37" s="17"/>
+      <c r="I37" s="17"/>
+      <c r="J37" s="17"/>
+      <c r="K37" s="17"/>
+      <c r="L37" s="18"/>
+      <c r="M37" s="17"/>
+      <c r="N37" s="17"/>
+      <c r="O37" s="17"/>
+      <c r="P37" s="17"/>
+      <c r="Q37" s="17"/>
+      <c r="R37" s="17"/>
+      <c r="S37" s="17"/>
+      <c r="T37" s="17"/>
+      <c r="U37" s="17"/>
+      <c r="V37" s="17"/>
+    </row>
+    <row r="38" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>1942</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C38" s="11"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+      <c r="K38" s="17"/>
+      <c r="L38" s="18"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="17"/>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="17"/>
+      <c r="S38" s="17"/>
+      <c r="T38" s="17"/>
+      <c r="U38" s="17"/>
+      <c r="V38" s="17"/>
+    </row>
+    <row r="39" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="12"/>
+      <c r="C39" s="13"/>
+      <c r="E39" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F39" s="6"/>
+      <c r="H39" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+      <c r="K39" s="17"/>
+      <c r="L39" s="18"/>
+      <c r="M39" s="17"/>
+      <c r="N39" s="17"/>
+      <c r="O39" s="17"/>
+      <c r="P39" s="17"/>
+      <c r="Q39" s="17"/>
+      <c r="R39" s="17"/>
+      <c r="S39" s="17"/>
+      <c r="T39" s="17"/>
+      <c r="U39" s="17"/>
+      <c r="V39" s="17"/>
+    </row>
+    <row r="40" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="C40" s="23"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+      <c r="K40" s="17"/>
+      <c r="L40" s="18"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="17"/>
+      <c r="P40" s="17"/>
+      <c r="Q40" s="17"/>
+      <c r="R40" s="17"/>
+      <c r="S40" s="17"/>
+      <c r="T40" s="17"/>
+      <c r="U40" s="17"/>
+      <c r="V40" s="17"/>
+    </row>
+    <row r="41" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B41" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" s="22"/>
+      <c r="E41" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F41" s="4"/>
+      <c r="H41" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="I41" s="20"/>
+      <c r="J41" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="K41" s="17"/>
+      <c r="L41" s="18"/>
+      <c r="M41" s="17"/>
+      <c r="N41" s="17"/>
+      <c r="O41" s="17"/>
+      <c r="P41" s="17"/>
+      <c r="Q41" s="17"/>
+      <c r="R41" s="17"/>
+      <c r="S41" s="17"/>
+      <c r="T41" s="17"/>
+      <c r="U41" s="17"/>
+      <c r="V41" s="17"/>
+    </row>
+    <row r="42" spans="1:22" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H42" s="20"/>
+      <c r="I42" s="20"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="17"/>
+      <c r="L42" s="18"/>
+      <c r="M42" s="17"/>
+      <c r="N42" s="17"/>
+      <c r="O42" s="17"/>
+      <c r="P42" s="17"/>
+      <c r="Q42" s="17"/>
+      <c r="R42" s="17"/>
+      <c r="S42" s="17"/>
+      <c r="T42" s="17"/>
+      <c r="U42" s="17"/>
+      <c r="V42" s="17"/>
+    </row>
+    <row r="43" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F43" s="4"/>
+      <c r="H43" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="I43" s="6"/>
+    </row>
+    <row r="44" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K44" s="16"/>
+      <c r="L44" s="18"/>
+      <c r="M44" s="17"/>
+      <c r="N44" s="17"/>
+      <c r="O44" s="17"/>
+      <c r="P44" s="17"/>
+      <c r="Q44" s="17"/>
+      <c r="R44" s="17"/>
+      <c r="S44" s="17"/>
+      <c r="T44" s="17"/>
+      <c r="U44" s="17"/>
+      <c r="V44" s="17"/>
+    </row>
+    <row r="45" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>1942</v>
+      </c>
+      <c r="C45" s="16"/>
+      <c r="D45" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="14"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="H45" s="17"/>
+      <c r="I45" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="J45" s="16"/>
+      <c r="K45" s="17"/>
+      <c r="L45" s="18"/>
+      <c r="M45" s="17"/>
+      <c r="N45" s="17"/>
+      <c r="O45" s="17"/>
+      <c r="P45" s="17"/>
+      <c r="Q45" s="17"/>
+      <c r="R45" s="17"/>
+      <c r="S45" s="17"/>
+      <c r="T45" s="17"/>
+      <c r="U45" s="17"/>
+      <c r="V45" s="17"/>
+    </row>
+    <row r="46" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+      <c r="K46" s="17"/>
+      <c r="L46" s="18"/>
+      <c r="M46" s="17"/>
+      <c r="N46" s="17"/>
+      <c r="O46" s="17"/>
+      <c r="P46" s="17"/>
+      <c r="Q46" s="17"/>
+      <c r="R46" s="17"/>
+      <c r="S46" s="17"/>
+      <c r="T46" s="17"/>
+      <c r="U46" s="17"/>
+      <c r="V46" s="17"/>
+    </row>
+    <row r="47" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E47" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F47" s="4"/>
+      <c r="M47" s="17"/>
+      <c r="N47" s="17"/>
+      <c r="O47" s="17"/>
+      <c r="P47" s="17"/>
+      <c r="Q47" s="17"/>
+      <c r="R47" s="17"/>
+      <c r="S47" s="17"/>
+      <c r="T47" s="17"/>
+      <c r="U47" s="17"/>
+      <c r="V47" s="17"/>
+    </row>
+    <row r="48" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H48" s="17"/>
+      <c r="I48" s="17"/>
+      <c r="J48" s="17"/>
+      <c r="K48" s="17"/>
+      <c r="L48" s="18"/>
+      <c r="M48" s="17"/>
+      <c r="N48" s="17"/>
+      <c r="O48" s="17"/>
+      <c r="P48" s="17"/>
+      <c r="Q48" s="17"/>
+      <c r="R48" s="17"/>
+      <c r="S48" s="17"/>
+      <c r="T48" s="17"/>
+      <c r="U48" s="17"/>
+      <c r="V48" s="17"/>
+    </row>
+    <row r="49" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>1942</v>
+      </c>
+      <c r="C49" s="16"/>
+      <c r="D49" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E49" s="14"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="J49" s="16"/>
+      <c r="K49" s="17"/>
+      <c r="L49" s="18"/>
+      <c r="M49" s="17"/>
+      <c r="N49" s="17"/>
+      <c r="O49" s="17"/>
+      <c r="P49" s="17"/>
+      <c r="Q49" s="17"/>
+      <c r="R49" s="17"/>
+      <c r="S49" s="17"/>
+      <c r="T49" s="17"/>
+      <c r="U49" s="17"/>
+      <c r="V49" s="17"/>
+    </row>
+    <row r="50" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+      <c r="K50" s="17"/>
+      <c r="L50" s="18"/>
+      <c r="M50" s="17"/>
+      <c r="N50" s="17"/>
+      <c r="O50" s="17"/>
+      <c r="P50" s="17"/>
+      <c r="Q50" s="17"/>
+      <c r="R50" s="17"/>
+      <c r="S50" s="17"/>
+      <c r="T50" s="17"/>
+      <c r="U50" s="17"/>
+      <c r="V50" s="17"/>
+    </row>
+    <row r="51" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>1943</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F51" s="4"/>
+      <c r="H51" s="17"/>
+      <c r="I51" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="J51" s="21"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="18"/>
+      <c r="M51" s="17"/>
+      <c r="N51" s="17"/>
+      <c r="O51" s="17"/>
+      <c r="P51" s="17"/>
+      <c r="Q51" s="17"/>
+      <c r="R51" s="17"/>
+      <c r="S51" s="17"/>
+      <c r="T51" s="17"/>
+      <c r="U51" s="17"/>
+      <c r="V51" s="17"/>
+    </row>
+    <row r="52" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H52" s="17"/>
+      <c r="I52" s="17"/>
+      <c r="J52" s="17"/>
+      <c r="K52" s="17"/>
+      <c r="L52" s="18"/>
+      <c r="M52" s="17"/>
+      <c r="N52" s="17"/>
+      <c r="O52" s="17"/>
+      <c r="P52" s="17"/>
+      <c r="Q52" s="17"/>
+      <c r="R52" s="17"/>
+      <c r="S52" s="17"/>
+      <c r="T52" s="17"/>
+      <c r="U52" s="17"/>
+      <c r="V52" s="17"/>
+    </row>
+    <row r="53" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>1943</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E53" s="14"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="H53" s="17"/>
+      <c r="I53" s="17"/>
+      <c r="J53" s="16"/>
+      <c r="K53" s="16"/>
+      <c r="L53" s="18"/>
+      <c r="M53" s="17"/>
+      <c r="N53" s="17"/>
+      <c r="O53" s="17"/>
+      <c r="P53" s="17"/>
+      <c r="Q53" s="17"/>
+      <c r="R53" s="17"/>
+      <c r="S53" s="17"/>
+      <c r="T53" s="17"/>
+      <c r="U53" s="17"/>
+      <c r="V53" s="17"/>
+    </row>
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="L54" s="2"/>
+    </row>
+    <row r="55" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>1944</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" s="11"/>
+      <c r="L55" s="2"/>
+    </row>
+    <row r="56" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="12"/>
+      <c r="C56" s="13"/>
+      <c r="E56" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F56" s="6"/>
+      <c r="I56" t="s">
+        <v>79</v>
+      </c>
+      <c r="L56" s="2"/>
+    </row>
+    <row r="57" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B57" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="C57" s="23"/>
+    </row>
+    <row r="58" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="22" t="s">
+        <v>77</v>
+      </c>
+      <c r="C58" s="22"/>
+      <c r="E58" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F58" s="4"/>
+      <c r="H58" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="I58" s="6"/>
+      <c r="K58" t="s">
+        <v>83</v>
+      </c>
+      <c r="N58" t="s">
+        <v>84</v>
+      </c>
+      <c r="O58" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="59" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="60" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E60" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F60" s="4"/>
+      <c r="H60" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="I60" s="6"/>
+    </row>
+    <row r="61" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>1944</v>
+      </c>
+      <c r="C62" s="16"/>
+      <c r="D62" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E62" s="14"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="15" t="s">
+        <v>80</v>
+      </c>
+      <c r="I62" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="64" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="65" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D65" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="E65" s="26"/>
+      <c r="F65" s="27"/>
+    </row>
+    <row r="66" spans="4:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D66" s="28"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="57">
+    <mergeCell ref="D65:F66"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="D62:F62"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="D49:F49"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="D53:F53"/>
+    <mergeCell ref="B55:C56"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="D45:F45"/>
+    <mergeCell ref="B25:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="D36:F36"/>
+    <mergeCell ref="H27:I27"/>
+    <mergeCell ref="B38:C39"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="B11:C12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B18:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="M38:N38"/>
+    <mergeCell ref="P38:Q38"/>
+    <mergeCell ref="M40:N40"/>
+    <mergeCell ref="D23:F23"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="D29:F29"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="P34:Q34"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="M36:N36"/>
+    <mergeCell ref="P36:Q36"/>
+    <mergeCell ref="B31:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>